<commit_message>
[UPDATE] Se realizan avances en la organización del repositorio e integración de los resultados obtenidos en los modelos [Proyecto TFM]
</commit_message>
<xml_diff>
--- a/Proyecto_TFM/Models/MotileDetection/ComparativaResultadoModelos.xlsx
+++ b/Proyecto_TFM/Models/MotileDetection/ComparativaResultadoModelos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unirioja-my.sharepoint.com/personal/migomesu_unirioja_es/Documents/RepositoriosPersonales/TrabajosMaestriaCienciadeDatos/Proyecto_TFM/ModelsTesting/ModelsForMotileSpermDetection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unirioja-my.sharepoint.com/personal/migomesu_unirioja_es/Documents/RepositoriosPersonales/TrabajosMaestriaCienciadeDatos/Proyecto_TFM/Models/MotileDetection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{34254ECE-FD1E-4201-8731-02D5183B4F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{605C2298-E04F-4FF0-B095-DAEBB2B94199}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{34254ECE-FD1E-4201-8731-02D5183B4F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39820DEE-B5AC-46CE-BABA-09A9E42AB5E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72723DD5-1670-4122-A76C-B523AB65F5B5}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,7 +112,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -129,36 +129,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EB7816-C12B-45E5-97E3-6B1A311334C0}">
   <dimension ref="B5:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="B5:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,254 +499,254 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>640</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>0.5</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>0.92</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>0.94</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3">
+      <c r="B7" s="6"/>
+      <c r="C7">
         <v>1200</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>0.97699999999999998</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>0.88</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>0.93</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3">
+      <c r="B8" s="6"/>
+      <c r="C8">
         <v>1920</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>1.167</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>0.93</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>0.94</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>640</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>0.45100000000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>0.9</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>0.93</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3">
+      <c r="B10" s="6"/>
+      <c r="C10">
         <v>1200</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>1.6850000000000001</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>0.91600000000000004</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <v>0.91</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="7">
+      <c r="B11" s="6"/>
+      <c r="C11" s="4">
         <v>1920</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="4">
         <v>2.0819999999999999</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="4">
         <v>0.96899999999999997</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="4">
         <v>0.94699999999999995</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>640</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>0.49299999999999999</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>0.91</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>0.92</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="6">
+      <c r="B13" s="6"/>
+      <c r="C13" s="3">
         <v>1200</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="3">
         <v>2.9420000000000002</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="3">
         <v>0.96</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="3">
         <v>0.94799999999999995</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3">
+      <c r="B14" s="6"/>
+      <c r="C14">
         <v>1920</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>3.887</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <v>0.94</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <v>0.96</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>640</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15">
         <v>0.71</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <v>0.86</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <v>0.96</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3">
+      <c r="B16" s="6"/>
+      <c r="C16">
         <v>1200</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16">
         <v>4.51</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
         <v>0.91</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>0.94</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3">
+      <c r="B17" s="6"/>
+      <c r="C17">
         <v>1920</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17">
         <v>5.7610000000000001</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>0.91200000000000003</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <v>0.94499999999999995</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>640</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>1.1419999999999999</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>0.89</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>0.89</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3">
+      <c r="B19" s="6"/>
+      <c r="C19">
         <v>1200</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19">
         <v>4.008</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>0.92100000000000004</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <v>0.92</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="5">
+      <c r="B20" s="7"/>
+      <c r="C20" s="2">
         <v>1920</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="2">
         <v>9.73</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="2">
         <v>0.95199999999999996</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="2">
         <v>0.90500000000000003</v>
       </c>
     </row>
@@ -777,5 +764,6 @@
     <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>